<commit_message>
Successfully implemented dynamic shift blocks and made a function to generate either static or dynamic shift blocks
TODO in the next commit: 1. Add dynamic shift block back to the front end for user to validate + error message if cannot find solution, 2. Steamline the shift blocks throughout both python files, very messy
</commit_message>
<xml_diff>
--- a/timetables/Normal Week of 230924.xlsx
+++ b/timetables/Normal Week of 230924.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
-  <si>
-    <t>DUTY 260924 THURSDAY</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
+  <si>
+    <t>DUTY 270924 FRIDAY</t>
   </si>
   <si>
     <t>0600-0700</t>
@@ -61,79 +61,79 @@
     <t>HAKIM</t>
   </si>
   <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
     <t>SENTRY</t>
   </si>
   <si>
+    <t>JIAN JUN</t>
+  </si>
+  <si>
+    <t>KAH FAI</t>
+  </si>
+  <si>
+    <t>DESK</t>
+  </si>
+  <si>
+    <t>DI ER</t>
+  </si>
+  <si>
+    <t>X-RAY</t>
+  </si>
+  <si>
+    <t>XAVIER</t>
+  </si>
+  <si>
+    <t>ANIQ</t>
+  </si>
+  <si>
+    <t>SCA1</t>
+  </si>
+  <si>
     <t>PAC</t>
   </si>
   <si>
-    <t>JIAN JUN</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>KAH FAI</t>
-  </si>
-  <si>
-    <t>SCA1</t>
-  </si>
-  <si>
-    <t>DI ER</t>
-  </si>
-  <si>
-    <t>DESK</t>
-  </si>
-  <si>
-    <t>OUT</t>
-  </si>
-  <si>
-    <t>XAVIER</t>
-  </si>
-  <si>
-    <t>X-RAY</t>
+    <t>JUN</t>
+  </si>
+  <si>
+    <t>ANIISH</t>
+  </si>
+  <si>
+    <t>SYAFI'I</t>
+  </si>
+  <si>
+    <t>JOSHUA</t>
+  </si>
+  <si>
+    <t>HILMI</t>
+  </si>
+  <si>
+    <t>SCA2</t>
+  </si>
+  <si>
+    <t>HUGO</t>
   </si>
   <si>
     <t>PROWL</t>
   </si>
   <si>
-    <t>ANIQ</t>
-  </si>
-  <si>
-    <t>JUN</t>
-  </si>
-  <si>
-    <t>ANIISH</t>
-  </si>
-  <si>
-    <t>SCA2</t>
-  </si>
-  <si>
-    <t>SYAFI'I</t>
-  </si>
-  <si>
-    <t>JOSHUA</t>
-  </si>
-  <si>
-    <t>HILMI</t>
-  </si>
-  <si>
-    <t>HUGO</t>
-  </si>
-  <si>
     <t>DHRUVA</t>
   </si>
   <si>
     <t>MARC</t>
   </si>
   <si>
-    <t>FLAG:JOSHUA // KAH FAI // ANIQ</t>
-  </si>
-  <si>
-    <t>LAST ENSURER: DI ER</t>
-  </si>
-  <si>
-    <t>BREAKFAST:MARC // DINNER:HUGO</t>
+    <t>FLAG:JOSHUA // XAVIER // KAH FAI</t>
+  </si>
+  <si>
+    <t>LAST ENSURER: ANIISH</t>
+  </si>
+  <si>
+    <t>BREAKFAST:JIAN JUN // DINNER:MARC</t>
   </si>
 </sst>
 </file>
@@ -194,25 +194,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF00FF"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,6 +213,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,7 +300,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -681,15 +681,17 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="7" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="K3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="4">
         <v>5</v>
@@ -701,24 +703,24 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
       <c r="N5" s="4">
         <v>5</v>
       </c>
@@ -732,21 +734,21 @@
         <v>19</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="M7" s="8"/>
       <c r="N7" s="4">
         <v>5</v>
       </c>
@@ -759,19 +761,19 @@
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="10" t="s">
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="G9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -787,28 +789,30 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="5"/>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="12"/>
+      <c r="J11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
       <c r="N11" s="4">
         <v>5</v>
       </c>
@@ -819,28 +823,26 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="H13" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="L13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="11"/>
       <c r="N13" s="4">
         <v>5</v>
       </c>
@@ -851,22 +853,22 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9" t="s">
         <v>22</v>
       </c>
+      <c r="E15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -883,32 +885,30 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="10" t="s">
+      <c r="H17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" s="6"/>
       <c r="N17" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -917,32 +917,30 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="10" t="s">
+      <c r="F19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="10" t="s">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="M19" s="10"/>
+      <c r="M19" s="9"/>
       <c r="N19" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -951,32 +949,32 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M21" s="8"/>
+      <c r="G21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -985,32 +983,30 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>18</v>
+      <c r="C23" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="M23" s="11"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
       <c r="N23" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1019,26 +1015,28 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="8" t="s">
-        <v>18</v>
+      <c r="F25" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K25" s="12"/>
-      <c r="L25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
       <c r="N25" s="4">
         <v>5</v>
       </c>
@@ -1051,24 +1049,22 @@
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="B27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I27" s="12"/>
-      <c r="J27" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K27" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="F27" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="4">
@@ -1083,24 +1079,26 @@
       <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="10" t="s">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
+      <c r="K29" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M29" s="4"/>
       <c r="N29" s="4">
         <v>5</v>
       </c>
@@ -1160,27 +1158,24 @@
       <c r="N32" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="20">
     <mergeCell ref="A1:N1"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="L7:M7"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="L13:M13"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="L17:M17"/>
     <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="L29:M29"/>
     <mergeCell ref="A30:C32"/>
     <mergeCell ref="K30:N32"/>
     <mergeCell ref="D30:J32"/>

</xml_diff>